<commit_message>
Save and Cancel buttons
</commit_message>
<xml_diff>
--- a/docs/Define merges and diffs.xlsx
+++ b/docs/Define merges and diffs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jan/Documents/Projects/Pragma-git/Pragma-git/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05006D93-4083-D440-88EA-74E1CCD4FAA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A9EE6E-1B65-6042-88B7-4CD02395E7F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2800" yWindow="8240" windowWidth="32840" windowHeight="20980" xr2:uid="{F41B7186-2348-6B4C-A6A8-C3BAD1CA00B3}"/>
   </bookViews>
@@ -602,7 +602,7 @@
   <dimension ref="B3:L37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E6" sqref="C6:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>